<commit_message>
Adding Pricing excel sheet and converted csv files
</commit_message>
<xml_diff>
--- a/DnD-WishList.xlsx
+++ b/DnD-WishList.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="-400" yWindow="20" windowWidth="28300" windowHeight="9780" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RankedWishList" sheetId="1" r:id="rId1"/>
+    <sheet name="Amazon" sheetId="2" r:id="rId2"/>
+    <sheet name="Local Shop" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Monster Manual</t>
   </si>
@@ -30,9 +32,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t># of pages/cards</t>
-  </si>
-  <si>
     <t>Sword Coast Adventurers Guide</t>
   </si>
   <si>
@@ -85,6 +84,18 @@
   </si>
   <si>
     <t>Kit</t>
+  </si>
+  <si>
+    <t>ProductID</t>
+  </si>
+  <si>
+    <t>NumberOfPagesCards</t>
+  </si>
+  <si>
+    <t>AmazonPrice</t>
+  </si>
+  <si>
+    <t>LocalShopPrice</t>
   </si>
 </sst>
 </file>
@@ -133,8 +144,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -143,11 +188,45 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -477,194 +556,562 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>27.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3">
+        <v>26.83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="B4">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="B5">
+        <v>34.729999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>14.98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>14.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>28.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B9">
+        <v>17.010000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>8.9499999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>12.96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>12.96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>14.68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>15.59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>12.49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>49.95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>39.950000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>49.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>15.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="B7">
+        <v>19.989999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="B8">
+        <v>49.95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>22.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+      <c r="B11">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+      <c r="B12">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+      <c r="B13">
+        <v>16.989999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+      <c r="B14">
+        <v>16.989999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+      <c r="B15">
+        <v>19.989999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+      <c r="B16">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>21</v>
+      <c r="B17">
+        <v>19.989999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>